<commit_message>
add tabel format baru
</commit_message>
<xml_diff>
--- a/010 Watubangga/Puskesmas 010 Watubangga.xlsx
+++ b/010 Watubangga/Puskesmas 010 Watubangga.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\kcda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\kcda-blanko-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B4CE7C-9A32-4534-A9E7-7BF0DC817DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7556835-F987-4FD0-B2BF-076781331F0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Bab 4" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -165,7 +165,10 @@
     <t>Sumber/Source:</t>
   </si>
   <si>
-    <t>Tabel 4.2.3</t>
+    <t>Kecamatan {kec}</t>
+  </si>
+  <si>
+    <t>Tabel 4.2.5</t>
   </si>
   <si>
     <r>
@@ -180,7 +183,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 4.2.4.</t>
+      <t xml:space="preserve"> 4.2.6.</t>
     </r>
   </si>
   <si>
@@ -196,41 +199,38 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 4.2.5.</t>
+      <t xml:space="preserve"> 4.2.7.</t>
     </r>
   </si>
   <si>
-    <t>Jumlah Tenaga Kesehatan Menurut Kelurahan/Desa in Kecamatan {kec}. 2020</t>
-  </si>
-  <si>
-    <t>Banyaknya Bayi yang Diimunisasi Menurut Jenis dan Desa/Kelurahan di Kecamatan {kec}, 2020</t>
-  </si>
-  <si>
-    <t>Banyaknya Ibu Melahirkan dan Kelahiran Ditolong Tenaga Kesehatan Menurut Desa/Kelurahan di Kecamatan {kec}, 2020</t>
-  </si>
-  <si>
-    <t>Banyaknya Pasangan Usia Subur dan Peserta KB Menurut Desa/Kelurahan di Kecamatan {kec}, 2020</t>
-  </si>
-  <si>
-    <t>Number of Medical Personnel by Kelurahan/ Village in {kec} Subdistrict, 2020</t>
-  </si>
-  <si>
-    <t>Number of Immunized Babies by Types of Immunization and Kelurahan/Village {kec} Subdistrict, 2020</t>
-  </si>
-  <si>
-    <t>Number of Woman Giving Brth and Birth Assisted by Paramedics by Kelurahan/Village in {kec} Subdistrict, 2020</t>
-  </si>
-  <si>
-    <t>Number of Fertile Age Couples and Family Planning Members by Kelurahan/Village in {kec} Subdistrict, 2020</t>
-  </si>
-  <si>
-    <t>Kecamatan {kec}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jumlah Tenaga Kesehatan Menurut Kelurahan/Desa in Kecamatan Watubangga. 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banyaknya Bayi yang Diimunisasi Menurut Jenis dan Desa/Kelurahan di Kecamatan Watubangga, 2020</t>
+    <t>Jumlah Tenaga Kesehatan Menurut Kelurahan/Desa in Kecamatan {kec}. 2021</t>
+  </si>
+  <si>
+    <t>Banyaknya Bayi yang Diimunisasi Menurut Jenis dan Desa/Kelurahan di Kecamatan {kec}, 2021</t>
+  </si>
+  <si>
+    <t>Banyaknya Ibu Melahirkan dan Kelahiran Ditolong Tenaga Kesehatan Menurut Desa/Kelurahan di Kecamatan {kec}, 2021</t>
+  </si>
+  <si>
+    <t>Banyaknya Pasangan Usia Subur dan Peserta KB Menurut Desa/Kelurahan di Kecamatan {kec}, 2021</t>
+  </si>
+  <si>
+    <t>Number of Medical Personnel by Kelurahan/ Village in {kec} Subdistrict, 2021</t>
+  </si>
+  <si>
+    <t>Number of Immunized Babies by Types of Immunization and Kelurahan/Village {kec} Subdistrict, 2021</t>
+  </si>
+  <si>
+    <t>Number of Woman Giving Brth and Birth Assisted by Paramedics by Kelurahan/Village in {kec} Subdistrict, 2021</t>
+  </si>
+  <si>
+    <t>Number of Fertile Age Couples and Family Planning Members by Kelurahan/Village in {kec} Subdistrict, 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumlah Tenaga Kesehatan Menurut Kelurahan/Desa in Kecamatan Watubangga. 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banyaknya Bayi yang Diimunisasi Menurut Jenis dan Desa/Kelurahan di Kecamatan Watubangga, 2021</t>
   </si>
   <si>
     <r>
@@ -245,11 +245,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 4.2.4.</t>
+      <t xml:space="preserve"> 4.2.6.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Banyaknya Ibu Melahirkan dan Kelahiran Ditolong Tenaga Kesehatan Menurut Desa/Kelurahan di Kecamatan Watubangga, 2020</t>
+    <t xml:space="preserve">Banyaknya Ibu Melahirkan dan Kelahiran Ditolong Tenaga Kesehatan Menurut Desa/Kelurahan di Kecamatan Watubangga, 2021</t>
   </si>
   <si>
     <r>
@@ -264,23 +264,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 4.2.5.</t>
+      <t xml:space="preserve"> 4.2.7.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Banyaknya Pasangan Usia Subur dan Peserta KB Menurut Desa/Kelurahan di Kecamatan Watubangga, 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of Medical Personnel by Kelurahan/ Village in Watubangga Subdistrict, 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of Immunized Babies by Types of Immunization and Kelurahan/Village Watubangga Subdistrict, 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of Woman Giving Brth and Birth Assisted by Paramedics by Kelurahan/Village in Watubangga Subdistrict, 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of Fertile Age Couples and Family Planning Members by Kelurahan/Village in Watubangga Subdistrict, 2020</t>
+    <t xml:space="preserve">Banyaknya Pasangan Usia Subur dan Peserta KB Menurut Desa/Kelurahan di Kecamatan Watubangga, 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Medical Personnel by Kelurahan/ Village in Watubangga Subdistrict, 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Immunized Babies by Types of Immunization and Kelurahan/Village Watubangga Subdistrict, 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Woman Giving Brth and Birth Assisted by Paramedics by Kelurahan/Village in Watubangga Subdistrict, 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Fertile Age Couples and Family Planning Members by Kelurahan/Village in Watubangga Subdistrict, 2021</t>
   </si>
   <si>
     <t xml:space="preserve">004 LONGGOSIPI</t>
@@ -913,9 +913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -952,7 +950,7 @@
       <c r="F1" s="40"/>
       <c r="G1" s="40"/>
       <c r="H1" t="s" s="22">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s" s="36">
         <v>44</v>

</xml_diff>